<commit_message>
updated geometry for initial RC finder
</commit_message>
<xml_diff>
--- a/Initial_RC_finder.xlsx
+++ b/Initial_RC_finder.xlsx
@@ -1,37 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joest\OneDrive\Documents\Work\FBR\VD\FBR_VD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryan/Documents/University/FBR/2019 VD scripts/FBR-VD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="11_06275381F1B9704E34D46C13CB95976A52C91669" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{5368A669-DC97-4CA6-AB0E-8E379EB8F49C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>x</t>
   </si>
@@ -84,23 +77,14 @@
     <t>c_rc</t>
   </si>
   <si>
-    <t>To plot graph:</t>
-  </si>
-  <si>
     <t>Initial roll centre</t>
-  </si>
-  <si>
-    <t>Stock</t>
-  </si>
-  <si>
-    <t>ANGLE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -108,13 +92,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -129,8 +127,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -164,7 +164,17 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.4845295417209536E-2"/>
+          <c:y val="1.2655575311150623E-2"/>
+          <c:w val="0.94667988443890561"/>
+          <c:h val="0.92120214811858192"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -228,7 +238,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-0AD5-4101-B4FB-63A3EB97E4B3}"/>
+                <c16:uniqueId val="{00000001-B3E0-0840-92EF-A9A6CD20BC65}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -261,7 +271,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000003-0AD5-4101-B4FB-63A3EB97E4B3}"/>
+                <c16:uniqueId val="{00000003-B3E0-0840-92EF-A9A6CD20BC65}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -287,7 +297,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>335</c:v>
+                  <c:v>348.38</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>351</c:v>
@@ -373,7 +383,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>149.9</c:v>
+                  <c:v>215.02</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>564.85</c:v>
@@ -388,7 +398,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>192</c:v>
+                  <c:v>149.15</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>171.5</c:v>
@@ -530,7 +540,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000007-0AD5-4101-B4FB-63A3EB97E4B3}"/>
+                <c16:uniqueId val="{00000007-B3E0-0840-92EF-A9A6CD20BC65}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -648,7 +658,7 @@
                   <c:v>538.53</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-975.36325184946918</c:v>
+                  <c:v>3976.309887408032</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -660,13 +670,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>335</c:v>
+                  <c:v>348.38</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>351</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>247.59199099388871</c:v>
+                  <c:v>389.45194375430782</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -716,13 +726,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>149.9</c:v>
+                  <c:v>215.02</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>564.85</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-975.36325184946918</c:v>
+                  <c:v>3976.309887408032</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -734,13 +744,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>192</c:v>
+                  <c:v>149.15</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>171.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>247.59199099388871</c:v>
+                  <c:v>389.45194375430782</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -887,7 +897,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-975.36325184946918</c:v>
+                  <c:v>3976.309887408032</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -902,10 +912,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>94.3</c:v>
+                  <c:v>-69.209999999999994</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>247.59199099388871</c:v>
+                  <c:v>389.45194375430782</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1665,15 +1675,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>177800</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>622300</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1997,70 +2007,53 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Q1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <v>304.29000000000002</v>
       </c>
       <c r="C2">
-        <v>335</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q2">
-        <v>304.29000000000002</v>
-      </c>
-      <c r="R2">
         <v>348.38</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3">
-        <v>149.9</v>
+        <v>215.02</v>
       </c>
       <c r="C3">
-        <v>192</v>
-      </c>
-      <c r="Q3">
-        <v>149.9</v>
-      </c>
-      <c r="R3">
-        <v>229.15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+        <v>149.15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B4">
@@ -2069,21 +2062,9 @@
       <c r="C4">
         <v>351</v>
       </c>
-      <c r="G4">
-        <v>304.29000000000002</v>
-      </c>
-      <c r="H4">
-        <v>348.38</v>
-      </c>
-      <c r="Q4">
-        <v>538.53</v>
-      </c>
-      <c r="R4">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B5">
@@ -2092,29 +2073,12 @@
       <c r="C5">
         <v>171.5</v>
       </c>
-      <c r="G5">
-        <v>538.53</v>
-      </c>
-      <c r="H5">
-        <v>351</v>
-      </c>
-      <c r="Q5">
-        <v>564.85</v>
-      </c>
-      <c r="R5">
-        <v>171.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="G6">
-        <v>149.9</v>
-      </c>
-      <c r="H6">
-        <v>229.15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7">
@@ -2123,15 +2087,9 @@
       <c r="C7">
         <v>0</v>
       </c>
-      <c r="G7">
-        <v>564.85</v>
-      </c>
-      <c r="H7">
-        <v>171.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B8">
@@ -2142,110 +2100,116 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B13">
         <f>((C4-C2)/(B4-B2))</f>
-        <v>6.8306010928961769E-2</v>
-      </c>
-      <c r="C13">
-        <f>ATAN((C4-C2)/(B4-B2))*(180/PI())</f>
-        <v>3.9075764766944241</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+        <v>1.1185109289617507E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B14">
         <f>((C5-C3)/(B5-B3))</f>
-        <v>-4.9403542595493427E-2</v>
-      </c>
-      <c r="C14">
-        <f>ATAN((C5-C3)/(B5-B3))*(180/PI())</f>
-        <v>-2.8283149472341318</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+        <v>6.3888174256067215E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B15">
         <f>C4-(B13*B4)</f>
-        <v>314.21516393442624</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+        <v>344.97648309426228</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B16">
         <f>C5-(B14*B5)</f>
-        <v>199.40559103506448</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+        <v>135.41276477146044</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B18">
         <f>(B16-B15)/(B13-B14)</f>
-        <v>-975.36325184946918</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+        <v>3976.309887408032</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B19">
         <f>((B13*B16)-(B14*B15))/(B13-B14)</f>
-        <v>247.59199099388871</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+        <v>389.45194375430782</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B21">
         <f>(B19-C8)/(B18-B8)</f>
-        <v>-0.15716501619751308</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+        <v>0.11534840009999414</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B22">
         <f>B19-(B21*B18)</f>
-        <v>94.299009718507875</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>18</v>
+        <v>-69.209040059996482</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="2"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="B24">
         <v>0</v>
       </c>
       <c r="C24">
         <f>ROUND(B22,2)</f>
-        <v>94.3</v>
+        <v>-69.209999999999994</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added some new aggressive geometries
</commit_message>
<xml_diff>
--- a/Initial_RC_finder.xlsx
+++ b/Initial_RC_finder.xlsx
@@ -1,23 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryan/Documents/University/FBR/2019 VD scripts/FBR-VD/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joest\OneDrive\Documents\Work\FBR\VD\FBR_VD\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="27" documentId="11_E62533E151B57BBE2A4C5E7B64FA4262CFEF6D20" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{A9F4AFCF-1CD8-4459-ACB7-7F983EFBE9EF}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -83,7 +90,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -282,10 +289,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>304.29000000000002</c:v>
+                  <c:v>305</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>538.53</c:v>
+                  <c:v>528</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -297,10 +304,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>348.38</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>351</c:v>
+                  <c:v>355</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -383,10 +390,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>215.02</c:v>
+                  <c:v>215</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>564.85</c:v>
+                  <c:v>565</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -398,10 +405,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>149.15</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>171.5</c:v>
+                  <c:v>140</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -450,10 +457,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>538.53</c:v>
+                  <c:v>528</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>564.85</c:v>
+                  <c:v>565</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -465,10 +472,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>351</c:v>
+                  <c:v>355</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>171.5</c:v>
+                  <c:v>140</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -554,7 +561,7 @@
                   <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>564.85</c:v>
+                  <c:v>565</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -569,7 +576,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>171.5</c:v>
+                  <c:v>140</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -652,13 +659,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>304.29000000000002</c:v>
+                  <c:v>305</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>538.53</c:v>
+                  <c:v>528</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3976.309887408032</c:v>
+                  <c:v>-249.9773755656108</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -670,13 +677,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>348.38</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>351</c:v>
+                  <c:v>355</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>389.45194375430782</c:v>
+                  <c:v>23.574660633484179</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -726,13 +733,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>215.02</c:v>
+                  <c:v>215</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>564.85</c:v>
+                  <c:v>565</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3976.309887408032</c:v>
+                  <c:v>-249.9773755656108</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -744,13 +751,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>149.15</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>171.5</c:v>
+                  <c:v>140</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>389.45194375430782</c:v>
+                  <c:v>23.574660633484179</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -897,7 +904,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3976.309887408032</c:v>
+                  <c:v>-249.9773755656108</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -912,10 +919,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-69.209999999999994</c:v>
+                  <c:v>16.64</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>389.45194375430782</c:v>
+                  <c:v>23.574660633484179</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2007,21 +2014,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -2030,54 +2037,54 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
-        <v>304.29000000000002</v>
+        <v>305</v>
       </c>
       <c r="C2">
-        <v>348.38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3">
-        <v>215.02</v>
+        <v>215</v>
       </c>
       <c r="C3">
-        <v>149.15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>538.53</v>
+        <v>528</v>
       </c>
       <c r="C4">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B5">
-        <v>564.85</v>
+        <v>565</v>
       </c>
       <c r="C5">
-        <v>171.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -2088,7 +2095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -2100,102 +2107,102 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B13">
         <f>((C4-C2)/(B4-B2))</f>
-        <v>1.1185109289617507E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>0.42600896860986548</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B14">
         <f>((C5-C3)/(B5-B3))</f>
-        <v>6.3888174256067215E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+        <v>0.14285714285714285</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B15">
         <f>C4-(B13*B4)</f>
-        <v>344.97648309426228</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+        <v>130.06726457399103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B16">
         <f>C5-(B14*B5)</f>
-        <v>135.41276477146044</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+        <v>59.285714285714292</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B18">
         <f>(B16-B15)/(B13-B14)</f>
-        <v>3976.309887408032</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+        <v>-249.9773755656108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B19">
         <f>((B13*B16)-(B14*B15))/(B13-B14)</f>
-        <v>389.45194375430782</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+        <v>23.574660633484179</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B21">
         <f>(B19-C8)/(B18-B8)</f>
-        <v>0.11534840009999414</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+        <v>-2.7735633101759447E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B22">
         <f>B19-(B21*B18)</f>
-        <v>-69.209040059996482</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+        <v>16.641379861055672</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>17</v>
       </c>
@@ -2204,7 +2211,7 @@
       </c>
       <c r="C24">
         <f>ROUND(B22,2)</f>
-        <v>-69.209999999999994</v>
+        <v>16.64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated geometries with new geometry tests
</commit_message>
<xml_diff>
--- a/Initial_RC_finder.xlsx
+++ b/Initial_RC_finder.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joest\OneDrive\Documents\Work\FBR\VD\FBR_VD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryan/Documents/University/FBR/2019 VD scripts/FBR-VD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79B3E3C-23CA-486D-8D4A-6CF4B4126CA6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>x</t>
   </si>
@@ -86,11 +85,23 @@
   <si>
     <t>Initial roll centre</t>
   </si>
+  <si>
+    <t>upper angle</t>
+  </si>
+  <si>
+    <t>uwb length</t>
+  </si>
+  <si>
+    <t>lower angle</t>
+  </si>
+  <si>
+    <t>lwb length</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -292,7 +303,7 @@
                   <c:v>305</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>528</c:v>
+                  <c:v>528.53</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -304,7 +315,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>290</c:v>
+                  <c:v>295</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>355</c:v>
@@ -393,7 +404,7 @@
                   <c:v>215</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>565</c:v>
+                  <c:v>564.85</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -457,10 +468,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>528</c:v>
+                  <c:v>528.53</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>565</c:v>
+                  <c:v>564.85</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -561,7 +572,7 @@
                   <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>565</c:v>
+                  <c:v>564.85</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -662,10 +673,10 @@
                   <c:v>305</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>528</c:v>
+                  <c:v>528.53</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-532.29140722291402</c:v>
+                  <c:v>-665.51007990843596</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -677,13 +688,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>290</c:v>
+                  <c:v>295</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>355</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45.946450809464508</c:v>
+                  <c:v>34.495348299976904</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -736,10 +747,10 @@
                   <c:v>215</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>565</c:v>
+                  <c:v>564.85</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-532.29140722291402</c:v>
+                  <c:v>-665.51007990843596</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -757,7 +768,7 @@
                   <c:v>140</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45.946450809464508</c:v>
+                  <c:v>34.495348299976904</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -904,7 +915,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-532.29140722291402</c:v>
+                  <c:v>-665.51007990843596</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -919,10 +930,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24.35</c:v>
+                  <c:v>16.350000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45.946450809464508</c:v>
+                  <c:v>34.495348299976904</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2014,21 +2025,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -2037,7 +2048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2045,10 +2056,10 @@
         <v>305</v>
       </c>
       <c r="C2">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -2059,32 +2070,32 @@
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>528</v>
+        <v>528.53</v>
       </c>
       <c r="C4">
         <v>355</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B5">
-        <v>565</v>
+        <v>564.85</v>
       </c>
       <c r="C5">
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -2095,7 +2106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -2107,102 +2118,102 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B13">
         <f>((C4-C2)/(B4-B2))</f>
-        <v>0.2914798206278027</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.2684203462622467</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B14">
         <f>((C5-C3)/(B5-B3))</f>
-        <v>8.5714285714285715E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8.5751036158353569E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B15">
         <f>C4-(B13*B4)</f>
-        <v>201.09865470852017</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>213.13179439001476</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B16">
         <f>C5-(B14*B5)</f>
-        <v>91.571428571428569</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>91.563527225953976</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B18">
         <f>(B16-B15)/(B13-B14)</f>
-        <v>-532.29140722291402</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-665.51007990843596</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B19">
         <f>((B13*B16)-(B14*B15))/(B13-B14)</f>
-        <v>45.946450809464508</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34.495348299976904</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B21">
         <f>(B19-C8)/(B18-B8)</f>
-        <v>-4.0578291521397226E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-2.725805890259899E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B22">
         <f>B19-(B21*B18)</f>
-        <v>24.346974912838338</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16.354835341559397</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>17</v>
       </c>
@@ -2211,7 +2222,43 @@
       </c>
       <c r="C24">
         <f>ROUND(B22,2)</f>
-        <v>24.35</v>
+        <v>16.350000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28">
+        <f>(ATAN((C4-C2)/(B4-B2)))*180/PI()</f>
+        <v>15.025183827484147</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29">
+        <f>SQRT(((C4-C2)^2)+((B4-B2)^2))</f>
+        <v>231.44256501343909</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30">
+        <f>(ATAN((C5-C3)/(B5-B3)))*180/PI()</f>
+        <v>4.9011827353718616</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31">
+        <f>SQRT(((C5-C3)^2)+((B5-B3)^2))</f>
+        <v>351.13390964132191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>